<commit_message>
Corrección títulos y descripciones de la escaleta
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado08/guion11/EscaletaCN_08_11_CO.xlsx
+++ b/fuentes/contenidos/grado08/guion11/EscaletaCN_08_11_CO.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GITHUB\CienciasNaturales\fuentes\contenidos\grado08\guion11\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="7755"/>
   </bookViews>
@@ -13,12 +18,12 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja2!$A$1:$U$53</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="144525" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="239">
   <si>
     <t>Asignatura</t>
   </si>
@@ -438,12 +443,6 @@
     <t>Timbre</t>
   </si>
   <si>
-    <t>Interactivo  con video que presenta las propiedades físicas del sonido.</t>
-  </si>
-  <si>
-    <t>Actividad para completar un texto sobre las diferentes características del sonido.</t>
-  </si>
-  <si>
     <t>Características del sonido</t>
   </si>
   <si>
@@ -453,24 +452,12 @@
     <t>El efecto doppler</t>
   </si>
   <si>
-    <t>Animación que describe el efecto doppler.  Un cambio en la percepción del sonido cuando el emisor se mueve.</t>
-  </si>
-  <si>
-    <t>Actividades que indagan sobre el concepto de sonidos y sus características.</t>
-  </si>
-  <si>
     <t>La luz</t>
   </si>
   <si>
     <t>Cálculo de la velocidad de la luz en diferentes medios.</t>
   </si>
   <si>
-    <t>Actividad que propone cálculos de la velocidad de la luz en diferentes medios.</t>
-  </si>
-  <si>
-    <t>En el interactivo observas las particularidades de que habla esta teoría. Compáralas con las teorías anteriores.</t>
-  </si>
-  <si>
     <t>La luz y la materia</t>
   </si>
   <si>
@@ -490,12 +477,6 @@
   </si>
   <si>
     <t>Actividad que permite identificar los elementos de la reflexión y refracción de la luz a partir de una imagen.</t>
-  </si>
-  <si>
-    <t>Actividad que propone un experimento para comprobar las principales características de la luz.</t>
-  </si>
-  <si>
-    <t>Actividad para  profundizar en los principales conceptos sobre las ondas.</t>
   </si>
   <si>
     <t xml:space="preserve">Cambiar el texto del segundo pantallazo, por el siguiente
@@ -506,9 +487,6 @@
 </t>
   </si>
   <si>
-    <t>Actividad que propone realizar un experimento para comprobar la descomposición de la luz blanca.</t>
-  </si>
-  <si>
     <t>Las ondas de luz y sonido</t>
   </si>
   <si>
@@ -557,9 +535,6 @@
     <t>El sonido: naturaleza y propagación</t>
   </si>
   <si>
-    <t>Actividad que permite reconocer las principales características del movimento circular uniforme y el oscilatorio</t>
-  </si>
-  <si>
     <t>Recurso F7-01</t>
   </si>
   <si>
@@ -614,9 +589,6 @@
     <t>Recurso M2A-01</t>
   </si>
   <si>
-    <t>Atividades sobre las ondas</t>
-  </si>
-  <si>
     <t xml:space="preserve">Refuerza tu aprendizaje: Las ondas  </t>
   </si>
   <si>
@@ -738,12 +710,48 @@
   </si>
   <si>
     <t>sI</t>
+  </si>
+  <si>
+    <t>Actividad que permite reconocer las principales características del movimiento circular uniforme y el oscilatorio</t>
+  </si>
+  <si>
+    <t>Refuerza tu aprendizaje: El movimiento periodico</t>
+  </si>
+  <si>
+    <t>Actividades sobre las ondas</t>
+  </si>
+  <si>
+    <t>Interactivo  con video que presenta las propiedades físicas del sonido</t>
+  </si>
+  <si>
+    <t>Actividad para completar un texto sobre las diferentes características del sonido</t>
+  </si>
+  <si>
+    <t>Animación que explica el efecto doppler</t>
+  </si>
+  <si>
+    <t>Actividades sobre las ondas sonoras</t>
+  </si>
+  <si>
+    <t>Interactivo que explica las propiedades de la luz</t>
+  </si>
+  <si>
+    <t>Actividad que propone cálculos de la velocidad de la luz en diferentes medios</t>
+  </si>
+  <si>
+    <t>Actividad que propone un experimento para comprobar las principales características de la luz</t>
+  </si>
+  <si>
+    <t>Actividad para  profundizar en los principales conceptos sobre las ondas</t>
+  </si>
+  <si>
+    <t>Actividad que propone realizar un experimento para comprobar la descomposición de la luz blanca</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1150,34 +1158,16 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1217,6 +1207,24 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1280,7 +1288,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1315,7 +1323,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1526,9 +1534,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:XFB132"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N5" sqref="N5"/>
+      <selection pane="bottomLeft" activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1557,94 +1565,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16382" s="42" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="98" t="s">
+      <c r="A1" s="92" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="96" t="s">
+      <c r="B1" s="90" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="107" t="s">
+      <c r="C1" s="101" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="98" t="s">
+      <c r="D1" s="92" t="s">
         <v>111</v>
       </c>
-      <c r="E1" s="96" t="s">
+      <c r="E1" s="90" t="s">
         <v>112</v>
       </c>
-      <c r="F1" s="94" t="s">
+      <c r="F1" s="86" t="s">
         <v>113</v>
       </c>
-      <c r="G1" s="100" t="s">
+      <c r="G1" s="94" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="94" t="s">
+      <c r="H1" s="86" t="s">
         <v>114</v>
       </c>
-      <c r="I1" s="94" t="s">
+      <c r="I1" s="86" t="s">
         <v>108</v>
       </c>
-      <c r="J1" s="104" t="s">
+      <c r="J1" s="98" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="102" t="s">
+      <c r="K1" s="96" t="s">
         <v>109</v>
       </c>
-      <c r="L1" s="100" t="s">
+      <c r="L1" s="94" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="106" t="s">
+      <c r="M1" s="100" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="106"/>
-      <c r="O1" s="86" t="s">
+      <c r="N1" s="100"/>
+      <c r="O1" s="88" t="s">
         <v>110</v>
       </c>
-      <c r="P1" s="86" t="s">
+      <c r="P1" s="88" t="s">
         <v>115</v>
       </c>
-      <c r="Q1" s="88" t="s">
+      <c r="Q1" s="103" t="s">
         <v>86</v>
       </c>
-      <c r="R1" s="92" t="s">
+      <c r="R1" s="107" t="s">
         <v>87</v>
       </c>
-      <c r="S1" s="88" t="s">
+      <c r="S1" s="103" t="s">
         <v>88</v>
       </c>
-      <c r="T1" s="90" t="s">
+      <c r="T1" s="105" t="s">
         <v>89</v>
       </c>
-      <c r="U1" s="88" t="s">
+      <c r="U1" s="103" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:16382" s="42" customFormat="1" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="99"/>
-      <c r="B2" s="97"/>
-      <c r="C2" s="108"/>
-      <c r="D2" s="99"/>
-      <c r="E2" s="97"/>
-      <c r="F2" s="95"/>
-      <c r="G2" s="101"/>
-      <c r="H2" s="95"/>
-      <c r="I2" s="95"/>
-      <c r="J2" s="105"/>
-      <c r="K2" s="103"/>
-      <c r="L2" s="101"/>
+      <c r="A2" s="93"/>
+      <c r="B2" s="91"/>
+      <c r="C2" s="102"/>
+      <c r="D2" s="93"/>
+      <c r="E2" s="91"/>
+      <c r="F2" s="87"/>
+      <c r="G2" s="95"/>
+      <c r="H2" s="87"/>
+      <c r="I2" s="87"/>
+      <c r="J2" s="99"/>
+      <c r="K2" s="97"/>
+      <c r="L2" s="95"/>
       <c r="M2" s="43" t="s">
         <v>91</v>
       </c>
       <c r="N2" s="43" t="s">
         <v>92</v>
       </c>
-      <c r="O2" s="87"/>
-      <c r="P2" s="87"/>
-      <c r="Q2" s="89"/>
-      <c r="R2" s="93"/>
-      <c r="S2" s="89"/>
-      <c r="T2" s="91"/>
-      <c r="U2" s="89"/>
+      <c r="O2" s="89"/>
+      <c r="P2" s="89"/>
+      <c r="Q2" s="104"/>
+      <c r="R2" s="108"/>
+      <c r="S2" s="104"/>
+      <c r="T2" s="106"/>
+      <c r="U2" s="104"/>
     </row>
     <row r="3" spans="1:16382" s="42" customFormat="1" ht="13.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
@@ -1654,15 +1662,15 @@
         <v>129</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>227</v>
+        <v>216</v>
       </c>
       <c r="D3" s="44" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="E3" s="45"/>
       <c r="F3" s="3"/>
       <c r="G3" s="30" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="H3" s="3">
         <v>1</v>
@@ -1671,7 +1679,7 @@
         <v>19</v>
       </c>
       <c r="J3" s="9" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="K3" s="10" t="s">
         <v>20</v>
@@ -1685,7 +1693,7 @@
       <c r="N3" s="12"/>
       <c r="O3" s="46"/>
       <c r="P3" s="46" t="s">
-        <v>237</v>
+        <v>226</v>
       </c>
       <c r="Q3" s="47">
         <v>6</v>
@@ -1697,7 +1705,7 @@
         <v>124</v>
       </c>
       <c r="T3" s="49" t="s">
-        <v>178</v>
+        <v>168</v>
       </c>
       <c r="U3" s="47" t="s">
         <v>125</v>
@@ -1711,17 +1719,17 @@
         <v>129</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>227</v>
+        <v>216</v>
       </c>
       <c r="D4" s="44" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="E4" s="45" t="s">
-        <v>228</v>
+        <v>217</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="35" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="H4" s="3">
         <v>2</v>
@@ -1730,7 +1738,7 @@
         <v>20</v>
       </c>
       <c r="J4" s="13" t="s">
-        <v>177</v>
+        <v>227</v>
       </c>
       <c r="K4" s="10" t="s">
         <v>20</v>
@@ -1744,22 +1752,22 @@
       </c>
       <c r="O4" s="46"/>
       <c r="P4" s="46" t="s">
-        <v>237</v>
+        <v>226</v>
       </c>
       <c r="Q4" s="47">
         <v>6</v>
       </c>
       <c r="R4" s="48" t="s">
+        <v>161</v>
+      </c>
+      <c r="S4" s="47" t="s">
+        <v>162</v>
+      </c>
+      <c r="T4" s="49" t="s">
         <v>170</v>
       </c>
-      <c r="S4" s="47" t="s">
-        <v>171</v>
-      </c>
-      <c r="T4" s="49" t="s">
-        <v>180</v>
-      </c>
       <c r="U4" s="47" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
     </row>
     <row r="5" spans="1:16382" s="42" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1770,17 +1778,17 @@
         <v>129</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>227</v>
+        <v>216</v>
       </c>
       <c r="D5" s="50" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="E5" s="51" t="s">
-        <v>229</v>
+        <v>218</v>
       </c>
       <c r="F5" s="52"/>
       <c r="G5" s="16" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="H5" s="3">
         <v>3</v>
@@ -1789,7 +1797,7 @@
         <v>20</v>
       </c>
       <c r="J5" s="18" t="s">
-        <v>185</v>
+        <v>175</v>
       </c>
       <c r="K5" s="19" t="s">
         <v>20</v>
@@ -1803,22 +1811,22 @@
       </c>
       <c r="O5" s="52"/>
       <c r="P5" s="52" t="s">
-        <v>237</v>
+        <v>226</v>
       </c>
       <c r="Q5" s="53">
         <v>6</v>
       </c>
       <c r="R5" s="54" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="S5" s="53" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="T5" s="85" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="U5" s="53" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
     </row>
     <row r="6" spans="1:16382" s="62" customFormat="1" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1829,17 +1837,17 @@
         <v>129</v>
       </c>
       <c r="C6" s="24" t="s">
-        <v>227</v>
+        <v>216</v>
       </c>
       <c r="D6" s="55" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="E6" s="56" t="s">
         <v>122</v>
       </c>
       <c r="F6" s="57"/>
       <c r="G6" s="25" t="s">
-        <v>164</v>
+        <v>228</v>
       </c>
       <c r="H6" s="26">
         <v>4</v>
@@ -1848,7 +1856,7 @@
         <v>20</v>
       </c>
       <c r="J6" s="58" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
       <c r="K6" s="27" t="s">
         <v>20</v>
@@ -1858,26 +1866,26 @@
       </c>
       <c r="M6" s="29"/>
       <c r="N6" s="29" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="O6" s="57"/>
       <c r="P6" s="57" t="s">
-        <v>237</v>
+        <v>226</v>
       </c>
       <c r="Q6" s="59">
         <v>6</v>
       </c>
       <c r="R6" s="60" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="S6" s="59" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="T6" s="61" t="s">
-        <v>189</v>
+        <v>179</v>
       </c>
       <c r="U6" s="59" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
     </row>
     <row r="7" spans="1:16382" s="42" customFormat="1" ht="13.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
@@ -1888,7 +1896,7 @@
         <v>129</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>227</v>
+        <v>216</v>
       </c>
       <c r="D7" s="63" t="s">
         <v>130</v>
@@ -1896,7 +1904,7 @@
       <c r="E7" s="64"/>
       <c r="F7" s="3"/>
       <c r="G7" s="4" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
       <c r="H7" s="3">
         <v>5</v>
@@ -1928,13 +1936,13 @@
         <v>127</v>
       </c>
       <c r="S7" s="66" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="T7" s="68" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="U7" s="66" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
     </row>
     <row r="8" spans="1:16382" s="42" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1945,7 +1953,7 @@
         <v>129</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>227</v>
+        <v>216</v>
       </c>
       <c r="D8" s="63" t="s">
         <v>130</v>
@@ -1964,7 +1972,7 @@
         <v>20</v>
       </c>
       <c r="J8" s="9" t="s">
-        <v>182</v>
+        <v>172</v>
       </c>
       <c r="K8" s="32" t="s">
         <v>20</v>
@@ -1978,22 +1986,22 @@
       </c>
       <c r="O8" s="69"/>
       <c r="P8" s="69" t="s">
-        <v>237</v>
+        <v>226</v>
       </c>
       <c r="Q8" s="47">
         <v>6</v>
       </c>
       <c r="R8" s="48" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="S8" s="47" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="T8" s="49" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="U8" s="47" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
     </row>
     <row r="9" spans="1:16382" s="70" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2004,7 +2012,7 @@
         <v>129</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>227</v>
+        <v>216</v>
       </c>
       <c r="D9" s="63" t="s">
         <v>130</v>
@@ -2014,7 +2022,7 @@
       </c>
       <c r="F9" s="69"/>
       <c r="G9" s="30" t="s">
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="H9" s="3">
         <v>7</v>
@@ -2023,7 +2031,7 @@
         <v>19</v>
       </c>
       <c r="J9" s="9" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="K9" s="32" t="s">
         <v>20</v>
@@ -2037,7 +2045,7 @@
       <c r="N9" s="34"/>
       <c r="O9" s="69"/>
       <c r="P9" s="69" t="s">
-        <v>237</v>
+        <v>226</v>
       </c>
       <c r="Q9" s="47">
         <v>6</v>
@@ -2049,7 +2057,7 @@
         <v>124</v>
       </c>
       <c r="T9" s="49" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="U9" s="47" t="s">
         <v>125</v>
@@ -2063,17 +2071,17 @@
         <v>129</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>227</v>
+        <v>216</v>
       </c>
       <c r="D10" s="63" t="s">
         <v>130</v>
       </c>
       <c r="E10" s="45" t="s">
-        <v>230</v>
+        <v>219</v>
       </c>
       <c r="F10" s="69"/>
       <c r="G10" s="30" t="s">
-        <v>193</v>
+        <v>183</v>
       </c>
       <c r="H10" s="3">
         <v>8</v>
@@ -2082,7 +2090,7 @@
         <v>20</v>
       </c>
       <c r="J10" s="9" t="s">
-        <v>194</v>
+        <v>184</v>
       </c>
       <c r="K10" s="32" t="s">
         <v>20</v>
@@ -2096,22 +2104,22 @@
       </c>
       <c r="O10" s="69"/>
       <c r="P10" s="69" t="s">
-        <v>237</v>
+        <v>226</v>
       </c>
       <c r="Q10" s="47">
         <v>6</v>
       </c>
       <c r="R10" s="48" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="S10" s="47" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="T10" s="49" t="s">
-        <v>195</v>
+        <v>185</v>
       </c>
       <c r="U10" s="47" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
     </row>
     <row r="11" spans="1:16382" s="71" customFormat="1" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2122,7 +2130,7 @@
         <v>129</v>
       </c>
       <c r="C11" s="24" t="s">
-        <v>227</v>
+        <v>216</v>
       </c>
       <c r="D11" s="55" t="s">
         <v>130</v>
@@ -2132,7 +2140,7 @@
       </c>
       <c r="F11" s="57"/>
       <c r="G11" s="25" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="H11" s="26">
         <v>9</v>
@@ -2141,7 +2149,7 @@
         <v>20</v>
       </c>
       <c r="J11" s="58" t="s">
-        <v>196</v>
+        <v>229</v>
       </c>
       <c r="K11" s="27" t="s">
         <v>19</v>
@@ -2162,13 +2170,13 @@
         <v>127</v>
       </c>
       <c r="S11" s="59" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="T11" s="61" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
       <c r="U11" s="59" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
     </row>
     <row r="12" spans="1:16382" s="42" customFormat="1" ht="13.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
@@ -2179,7 +2187,7 @@
         <v>129</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>227</v>
+        <v>216</v>
       </c>
       <c r="D12" s="63" t="s">
         <v>136</v>
@@ -2191,7 +2199,7 @@
         <v>138</v>
       </c>
       <c r="G12" s="35" t="s">
-        <v>231</v>
+        <v>220</v>
       </c>
       <c r="H12" s="3">
         <v>10</v>
@@ -2200,7 +2208,7 @@
         <v>19</v>
       </c>
       <c r="J12" s="13" t="s">
-        <v>139</v>
+        <v>230</v>
       </c>
       <c r="K12" s="10" t="s">
         <v>19</v>
@@ -2223,13 +2231,13 @@
         <v>127</v>
       </c>
       <c r="S12" s="66" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="T12" s="68" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="U12" s="66" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="V12" s="73"/>
       <c r="W12" s="73"/>
@@ -18601,7 +18609,7 @@
         <v>129</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>227</v>
+        <v>216</v>
       </c>
       <c r="D13" s="44" t="s">
         <v>136</v>
@@ -18613,7 +18621,7 @@
         <v>138</v>
       </c>
       <c r="G13" s="30" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="H13" s="3">
         <v>11</v>
@@ -18622,7 +18630,7 @@
         <v>20</v>
       </c>
       <c r="J13" s="9" t="s">
-        <v>140</v>
+        <v>231</v>
       </c>
       <c r="K13" s="32" t="s">
         <v>19</v>
@@ -18642,16 +18650,16 @@
         <v>8</v>
       </c>
       <c r="R13" s="48" t="s">
-        <v>198</v>
+        <v>187</v>
       </c>
       <c r="S13" s="47" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="T13" s="49" t="s">
-        <v>200</v>
+        <v>189</v>
       </c>
       <c r="U13" s="47" t="s">
-        <v>201</v>
+        <v>190</v>
       </c>
     </row>
     <row r="14" spans="1:16382" s="42" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -18662,17 +18670,17 @@
         <v>129</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>227</v>
+        <v>216</v>
       </c>
       <c r="D14" s="44" t="s">
         <v>136</v>
       </c>
       <c r="E14" s="45" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="F14" s="69"/>
       <c r="G14" s="30" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="H14" s="3">
         <v>12</v>
@@ -18681,7 +18689,7 @@
         <v>19</v>
       </c>
       <c r="J14" s="9" t="s">
-        <v>144</v>
+        <v>232</v>
       </c>
       <c r="K14" s="32" t="s">
         <v>19</v>
@@ -18701,16 +18709,16 @@
         <v>8</v>
       </c>
       <c r="R14" s="48" t="s">
-        <v>198</v>
+        <v>187</v>
       </c>
       <c r="S14" s="47" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="T14" s="49" t="s">
-        <v>202</v>
+        <v>191</v>
       </c>
       <c r="U14" s="47" t="s">
-        <v>201</v>
+        <v>190</v>
       </c>
     </row>
     <row r="15" spans="1:16382" s="42" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -18721,17 +18729,17 @@
         <v>129</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>227</v>
+        <v>216</v>
       </c>
       <c r="D15" s="44" t="s">
         <v>136</v>
       </c>
       <c r="E15" s="45" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="F15" s="69"/>
       <c r="G15" s="30" t="s">
-        <v>204</v>
+        <v>193</v>
       </c>
       <c r="H15" s="3">
         <v>13</v>
@@ -18740,7 +18748,7 @@
         <v>20</v>
       </c>
       <c r="J15" s="9" t="s">
-        <v>203</v>
+        <v>192</v>
       </c>
       <c r="K15" s="32" t="s">
         <v>20</v>
@@ -18760,16 +18768,16 @@
         <v>6</v>
       </c>
       <c r="R15" s="48" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="S15" s="47" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="T15" s="49" t="s">
-        <v>205</v>
+        <v>194</v>
       </c>
       <c r="U15" s="47" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
     </row>
     <row r="16" spans="1:16382" s="74" customFormat="1" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -18780,7 +18788,7 @@
         <v>129</v>
       </c>
       <c r="C16" s="38" t="s">
-        <v>227</v>
+        <v>216</v>
       </c>
       <c r="D16" s="55" t="s">
         <v>136</v>
@@ -18790,7 +18798,7 @@
       </c>
       <c r="F16" s="57"/>
       <c r="G16" s="25" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="H16" s="39">
         <v>14</v>
@@ -18799,7 +18807,7 @@
         <v>20</v>
       </c>
       <c r="J16" s="58" t="s">
-        <v>145</v>
+        <v>233</v>
       </c>
       <c r="K16" s="27" t="s">
         <v>19</v>
@@ -18810,7 +18818,7 @@
       <c r="M16" s="29"/>
       <c r="N16" s="29"/>
       <c r="O16" s="57" t="s">
-        <v>206</v>
+        <v>195</v>
       </c>
       <c r="P16" s="57" t="s">
         <v>19</v>
@@ -18819,16 +18827,16 @@
         <v>8</v>
       </c>
       <c r="R16" s="60" t="s">
-        <v>198</v>
+        <v>187</v>
       </c>
       <c r="S16" s="59" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="T16" s="61" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="U16" s="59" t="s">
-        <v>201</v>
+        <v>190</v>
       </c>
     </row>
     <row r="17" spans="1:21" s="42" customFormat="1" ht="13.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
@@ -18839,15 +18847,15 @@
         <v>129</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>227</v>
+        <v>216</v>
       </c>
       <c r="D17" s="63" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="E17" s="64"/>
       <c r="F17" s="46"/>
       <c r="G17" s="35" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="H17" s="3">
         <v>15</v>
@@ -18856,7 +18864,7 @@
         <v>19</v>
       </c>
       <c r="J17" s="13" t="s">
-        <v>149</v>
+        <v>234</v>
       </c>
       <c r="K17" s="10" t="s">
         <v>19</v>
@@ -18876,16 +18884,16 @@
         <v>5</v>
       </c>
       <c r="R17" s="67" t="s">
-        <v>208</v>
+        <v>197</v>
       </c>
       <c r="S17" s="66" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="T17" s="68" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="U17" s="66" t="s">
-        <v>209</v>
+        <v>198</v>
       </c>
     </row>
     <row r="18" spans="1:21" s="42" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -18896,17 +18904,17 @@
         <v>129</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>227</v>
+        <v>216</v>
       </c>
       <c r="D18" s="44" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="E18" s="64" t="s">
-        <v>232</v>
+        <v>221</v>
       </c>
       <c r="F18" s="46"/>
       <c r="G18" s="35" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
       <c r="H18" s="3">
         <v>16</v>
@@ -18915,7 +18923,7 @@
         <v>20</v>
       </c>
       <c r="J18" s="13" t="s">
-        <v>224</v>
+        <v>213</v>
       </c>
       <c r="K18" s="10" t="s">
         <v>20</v>
@@ -18929,22 +18937,22 @@
       </c>
       <c r="O18" s="46"/>
       <c r="P18" s="46" t="s">
-        <v>237</v>
+        <v>226</v>
       </c>
       <c r="Q18" s="47">
         <v>6</v>
       </c>
       <c r="R18" s="48" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="S18" s="47" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="T18" s="49" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
       <c r="U18" s="47" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
     </row>
     <row r="19" spans="1:21" s="42" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -18955,17 +18963,17 @@
         <v>129</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>227</v>
+        <v>216</v>
       </c>
       <c r="D19" s="63" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="E19" s="64" t="s">
-        <v>232</v>
+        <v>221</v>
       </c>
       <c r="F19" s="46"/>
       <c r="G19" s="35" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="H19" s="3">
         <v>17</v>
@@ -18974,7 +18982,7 @@
         <v>20</v>
       </c>
       <c r="J19" s="13" t="s">
-        <v>148</v>
+        <v>235</v>
       </c>
       <c r="K19" s="10" t="s">
         <v>19</v>
@@ -18994,16 +19002,16 @@
         <v>8</v>
       </c>
       <c r="R19" s="48" t="s">
-        <v>198</v>
+        <v>187</v>
       </c>
       <c r="S19" s="47" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="T19" s="49" t="s">
-        <v>207</v>
+        <v>196</v>
       </c>
       <c r="U19" s="47" t="s">
-        <v>201</v>
+        <v>190</v>
       </c>
     </row>
     <row r="20" spans="1:21" s="42" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -19014,17 +19022,17 @@
         <v>129</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>227</v>
+        <v>216</v>
       </c>
       <c r="D20" s="44" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="E20" s="45" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="F20" s="69"/>
       <c r="G20" s="30" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="H20" s="3">
         <v>18</v>
@@ -19033,7 +19041,7 @@
         <v>20</v>
       </c>
       <c r="J20" s="9" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="K20" s="32" t="s">
         <v>19</v>
@@ -19053,16 +19061,16 @@
         <v>8</v>
       </c>
       <c r="R20" s="48" t="s">
-        <v>198</v>
+        <v>187</v>
       </c>
       <c r="S20" s="47" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="T20" s="49" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="U20" s="47" t="s">
-        <v>201</v>
+        <v>190</v>
       </c>
     </row>
     <row r="21" spans="1:21" s="74" customFormat="1" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -19073,17 +19081,17 @@
         <v>129</v>
       </c>
       <c r="C21" s="38" t="s">
-        <v>227</v>
+        <v>216</v>
       </c>
       <c r="D21" s="55" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="E21" s="56" t="s">
         <v>122</v>
       </c>
       <c r="F21" s="57"/>
       <c r="G21" s="25" t="s">
-        <v>210</v>
+        <v>199</v>
       </c>
       <c r="H21" s="39">
         <v>19</v>
@@ -19092,7 +19100,7 @@
         <v>20</v>
       </c>
       <c r="J21" s="58" t="s">
-        <v>211</v>
+        <v>200</v>
       </c>
       <c r="K21" s="27" t="s">
         <v>19</v>
@@ -19112,16 +19120,16 @@
         <v>8</v>
       </c>
       <c r="R21" s="60" t="s">
-        <v>198</v>
+        <v>187</v>
       </c>
       <c r="S21" s="59" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="T21" s="61" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="U21" s="59" t="s">
-        <v>201</v>
+        <v>190</v>
       </c>
     </row>
     <row r="22" spans="1:21" ht="13.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
@@ -19132,17 +19140,17 @@
         <v>129</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>227</v>
+        <v>216</v>
       </c>
       <c r="D22" s="63" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="E22" s="64" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="F22" s="46"/>
       <c r="G22" s="35" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="H22" s="3">
         <v>20</v>
@@ -19151,7 +19159,7 @@
         <v>19</v>
       </c>
       <c r="J22" s="13" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="K22" s="10" t="s">
         <v>19</v>
@@ -19169,16 +19177,16 @@
         <v>8</v>
       </c>
       <c r="R22" s="67" t="s">
-        <v>198</v>
+        <v>187</v>
       </c>
       <c r="S22" s="66" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="T22" s="68" t="s">
-        <v>212</v>
+        <v>201</v>
       </c>
       <c r="U22" s="66" t="s">
-        <v>201</v>
+        <v>190</v>
       </c>
     </row>
     <row r="23" spans="1:21" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -19189,17 +19197,17 @@
         <v>129</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>227</v>
+        <v>216</v>
       </c>
       <c r="D23" s="63" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="E23" s="45" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="F23" s="69"/>
       <c r="G23" s="30" t="s">
-        <v>213</v>
+        <v>202</v>
       </c>
       <c r="H23" s="3">
         <v>21</v>
@@ -19208,7 +19216,7 @@
         <v>20</v>
       </c>
       <c r="J23" s="9" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="K23" s="32" t="s">
         <v>19</v>
@@ -19226,16 +19234,16 @@
         <v>8</v>
       </c>
       <c r="R23" s="48" t="s">
-        <v>198</v>
+        <v>187</v>
       </c>
       <c r="S23" s="47" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="T23" s="49" t="s">
-        <v>213</v>
+        <v>202</v>
       </c>
       <c r="U23" s="47" t="s">
-        <v>201</v>
+        <v>190</v>
       </c>
     </row>
     <row r="24" spans="1:21" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -19246,17 +19254,17 @@
         <v>129</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>227</v>
+        <v>216</v>
       </c>
       <c r="D24" s="63" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="E24" s="45" t="s">
-        <v>233</v>
+        <v>222</v>
       </c>
       <c r="F24" s="69"/>
       <c r="G24" s="30" t="s">
-        <v>214</v>
+        <v>203</v>
       </c>
       <c r="H24" s="3">
         <v>22</v>
@@ -19265,7 +19273,7 @@
         <v>20</v>
       </c>
       <c r="J24" s="9" t="s">
-        <v>215</v>
+        <v>204</v>
       </c>
       <c r="K24" s="32" t="s">
         <v>20</v>
@@ -19285,16 +19293,16 @@
         <v>6</v>
       </c>
       <c r="R24" s="48" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="S24" s="47" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="T24" s="49" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="U24" s="47" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
     </row>
     <row r="25" spans="1:21" s="74" customFormat="1" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -19305,17 +19313,17 @@
         <v>129</v>
       </c>
       <c r="C25" s="38" t="s">
-        <v>227</v>
+        <v>216</v>
       </c>
       <c r="D25" s="77" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="E25" s="56" t="s">
         <v>122</v>
       </c>
       <c r="F25" s="57"/>
       <c r="G25" s="25" t="s">
-        <v>216</v>
+        <v>205</v>
       </c>
       <c r="H25" s="39">
         <v>23</v>
@@ -19324,7 +19332,7 @@
         <v>20</v>
       </c>
       <c r="J25" s="78" t="s">
-        <v>217</v>
+        <v>206</v>
       </c>
       <c r="K25" s="27" t="s">
         <v>20</v>
@@ -19334,7 +19342,7 @@
       </c>
       <c r="M25" s="29"/>
       <c r="N25" s="29" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="O25" s="57"/>
       <c r="P25" s="57" t="s">
@@ -19344,16 +19352,16 @@
         <v>6</v>
       </c>
       <c r="R25" s="60" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="S25" s="59" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="T25" s="61" t="s">
-        <v>218</v>
+        <v>207</v>
       </c>
       <c r="U25" s="59" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
     </row>
     <row r="26" spans="1:21" ht="13.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
@@ -19364,7 +19372,7 @@
         <v>129</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>227</v>
+        <v>216</v>
       </c>
       <c r="D26" s="63" t="s">
         <v>128</v>
@@ -19372,7 +19380,7 @@
       <c r="E26" s="64"/>
       <c r="F26" s="46"/>
       <c r="G26" s="35" t="s">
-        <v>219</v>
+        <v>208</v>
       </c>
       <c r="H26" s="3">
         <v>24</v>
@@ -19381,7 +19389,7 @@
         <v>20</v>
       </c>
       <c r="J26" s="13" t="s">
-        <v>157</v>
+        <v>236</v>
       </c>
       <c r="K26" s="10" t="s">
         <v>19</v>
@@ -19401,16 +19409,16 @@
         <v>8</v>
       </c>
       <c r="R26" s="67" t="s">
-        <v>198</v>
+        <v>187</v>
       </c>
       <c r="S26" s="66" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="T26" s="68" t="s">
-        <v>219</v>
+        <v>208</v>
       </c>
       <c r="U26" s="66" t="s">
-        <v>201</v>
+        <v>190</v>
       </c>
     </row>
     <row r="27" spans="1:21" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -19421,7 +19429,7 @@
         <v>129</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>227</v>
+        <v>216</v>
       </c>
       <c r="D27" s="44" t="s">
         <v>128</v>
@@ -19429,7 +19437,7 @@
       <c r="E27" s="45"/>
       <c r="F27" s="69"/>
       <c r="G27" s="5" t="s">
-        <v>220</v>
+        <v>209</v>
       </c>
       <c r="H27" s="3">
         <v>25</v>
@@ -19438,7 +19446,7 @@
         <v>20</v>
       </c>
       <c r="J27" s="9" t="s">
-        <v>158</v>
+        <v>237</v>
       </c>
       <c r="K27" s="32" t="s">
         <v>19</v>
@@ -19449,7 +19457,7 @@
       <c r="M27" s="34"/>
       <c r="N27" s="34"/>
       <c r="O27" s="69" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="P27" s="46" t="s">
         <v>19</v>
@@ -19461,13 +19469,13 @@
         <v>127</v>
       </c>
       <c r="S27" s="47" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="T27" s="49" t="s">
-        <v>220</v>
+        <v>209</v>
       </c>
       <c r="U27" s="47" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
     </row>
     <row r="28" spans="1:21" s="74" customFormat="1" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -19478,7 +19486,7 @@
         <v>129</v>
       </c>
       <c r="C28" s="38" t="s">
-        <v>227</v>
+        <v>216</v>
       </c>
       <c r="D28" s="55" t="s">
         <v>128</v>
@@ -19486,7 +19494,7 @@
       <c r="E28" s="56"/>
       <c r="F28" s="57"/>
       <c r="G28" s="25" t="s">
-        <v>221</v>
+        <v>210</v>
       </c>
       <c r="H28" s="39">
         <v>26</v>
@@ -19495,7 +19503,7 @@
         <v>20</v>
       </c>
       <c r="J28" s="58" t="s">
-        <v>160</v>
+        <v>238</v>
       </c>
       <c r="K28" s="27" t="s">
         <v>19</v>
@@ -19518,13 +19526,13 @@
         <v>127</v>
       </c>
       <c r="S28" s="59" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="T28" s="61" t="s">
-        <v>221</v>
+        <v>210</v>
       </c>
       <c r="U28" s="59" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
     </row>
     <row r="29" spans="1:21" ht="13.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
@@ -19535,10 +19543,10 @@
         <v>129</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>227</v>
+        <v>216</v>
       </c>
       <c r="D29" s="63" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="E29" s="64"/>
       <c r="F29" s="46"/>
@@ -19552,7 +19560,7 @@
         <v>20</v>
       </c>
       <c r="J29" s="13" t="s">
-        <v>234</v>
+        <v>223</v>
       </c>
       <c r="K29" s="10" t="s">
         <v>20</v>
@@ -19580,15 +19588,15 @@
         <v>129</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>227</v>
+        <v>216</v>
       </c>
       <c r="D30" s="44" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="E30" s="45"/>
       <c r="F30" s="69"/>
       <c r="G30" s="80" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="H30" s="3">
         <v>28</v>
@@ -19597,7 +19605,7 @@
         <v>20</v>
       </c>
       <c r="J30" s="9" t="s">
-        <v>235</v>
+        <v>224</v>
       </c>
       <c r="K30" s="32" t="s">
         <v>20</v>
@@ -19617,16 +19625,16 @@
         <v>6</v>
       </c>
       <c r="R30" s="48" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="S30" s="47" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="T30" s="49" t="s">
-        <v>222</v>
+        <v>211</v>
       </c>
       <c r="U30" s="47" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
     </row>
     <row r="31" spans="1:21" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -19637,15 +19645,15 @@
         <v>129</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>227</v>
+        <v>216</v>
       </c>
       <c r="D31" s="44" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="E31" s="45"/>
       <c r="F31" s="69"/>
       <c r="G31" s="81" t="s">
-        <v>226</v>
+        <v>215</v>
       </c>
       <c r="H31" s="3">
         <v>29</v>
@@ -19654,7 +19662,7 @@
         <v>20</v>
       </c>
       <c r="J31" s="9" t="s">
-        <v>236</v>
+        <v>225</v>
       </c>
       <c r="K31" s="32" t="s">
         <v>20</v>
@@ -19674,16 +19682,16 @@
         <v>6</v>
       </c>
       <c r="R31" s="48" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="S31" s="47" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="T31" s="49" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="U31" s="47" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
     </row>
     <row r="32" spans="1:21" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -21023,6 +21031,12 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="O1:O2"/>
@@ -21037,12 +21051,6 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="F1:F2"/>
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="O12" r:id="rId1" display="http://hispanicasaber.planetasaber.com/encyclopedia/default.asp?idpack=5&amp;idpil=AN001065&amp;ruta=Buscador"/>

</xml_diff>